<commit_message>
Added the option to set to on/off each deck
</commit_message>
<xml_diff>
--- a/exampledeck.xlsx
+++ b/exampledeck.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="283">
   <si>
     <t>name</t>
   </si>
@@ -875,6 +875,12 @@
   </si>
   <si>
     <t>pink-petaled-flower</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>default</t>
   </si>
 </sst>
 </file>
@@ -1246,95 +1252,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>265</v>
       </c>
       <c r="B1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C1" t="s">
         <v>268</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
       <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>266</v>
       </c>
       <c r="B2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C2" t="s">
         <v>269</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>278</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>266</v>
       </c>
       <c r="B3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C3" t="s">
         <v>272</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>279</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>267</v>
       </c>
       <c r="B4" t="s">
+        <v>281</v>
+      </c>
+      <c r="C4" t="s">
         <v>271</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>280</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>267</v>
       </c>
       <c r="B5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C5" t="s">
         <v>270</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>277</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>274</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" display="https://www.pexels.com/es-es/foto/flor-flora-floracion-fondo-de-pantalla-de-flores-2187618/"/>
-    <hyperlink ref="D2" r:id="rId2" display="https://www.pexels.com/es-es/foto/dalia-flor-flora-floracion-863963/"/>
-    <hyperlink ref="D3" r:id="rId3" display="https://www.pexels.com/es-es/foto/flor-flora-floracion-fondo-de-pantalla-gratis-2039606/"/>
-    <hyperlink ref="D4" r:id="rId4" display="https://www.pexels.com/es-es/foto/estambre-flor-flora-floracion-2375010/"/>
+    <hyperlink ref="E5" r:id="rId1" display="https://www.pexels.com/es-es/foto/flor-flora-floracion-fondo-de-pantalla-de-flores-2187618/"/>
+    <hyperlink ref="E2" r:id="rId2" display="https://www.pexels.com/es-es/foto/dalia-flor-flora-floracion-863963/"/>
+    <hyperlink ref="E3" r:id="rId3" display="https://www.pexels.com/es-es/foto/flor-flora-floracion-fondo-de-pantalla-gratis-2039606/"/>
+    <hyperlink ref="E4" r:id="rId4" display="https://www.pexels.com/es-es/foto/estambre-flor-flora-floracion-2375010/"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
Rewriten module creation to divide between different decks
</commit_message>
<xml_diff>
--- a/exampledeck.xlsx
+++ b/exampledeck.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\R\sw-deck-customizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2086DDBF-B6DD-4024-9E68-F6ECB3C71E13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20370" windowHeight="12210"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="20376" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja2!$A$1:$C$109</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="284">
   <si>
     <t>name</t>
   </si>
@@ -881,12 +882,15 @@
   </si>
   <si>
     <t>default</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -940,7 +944,7 @@
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1251,22 +1255,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>265</v>
       </c>
@@ -1283,7 +1287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>266</v>
       </c>
@@ -1300,7 +1304,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>266</v>
       </c>
@@ -1317,12 +1321,12 @@
         <v>276</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>267</v>
       </c>
       <c r="B4" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C4" t="s">
         <v>271</v>
@@ -1334,12 +1338,12 @@
         <v>275</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>267</v>
       </c>
       <c r="B5" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C5" t="s">
         <v>270</v>
@@ -1353,10 +1357,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1" display="https://www.pexels.com/es-es/foto/flor-flora-floracion-fondo-de-pantalla-de-flores-2187618/"/>
-    <hyperlink ref="E2" r:id="rId2" display="https://www.pexels.com/es-es/foto/dalia-flor-flora-floracion-863963/"/>
-    <hyperlink ref="E3" r:id="rId3" display="https://www.pexels.com/es-es/foto/flor-flora-floracion-fondo-de-pantalla-gratis-2039606/"/>
-    <hyperlink ref="E4" r:id="rId4" display="https://www.pexels.com/es-es/foto/estambre-flor-flora-floracion-2375010/"/>
+    <hyperlink ref="E5" r:id="rId1" display="https://www.pexels.com/es-es/foto/flor-flora-floracion-fondo-de-pantalla-de-flores-2187618/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" display="https://www.pexels.com/es-es/foto/dalia-flor-flora-floracion-863963/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E3" r:id="rId3" display="https://www.pexels.com/es-es/foto/flor-flora-floracion-fondo-de-pantalla-gratis-2039606/" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E4" r:id="rId4" display="https://www.pexels.com/es-es/foto/estambre-flor-flora-floracion-2375010/" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -1364,21 +1368,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1390,7 +1394,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1402,7 +1406,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1414,7 +1418,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1426,7 +1430,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1438,7 +1442,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1450,7 +1454,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1462,7 +1466,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1474,7 +1478,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1486,7 +1490,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1498,7 +1502,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1510,7 +1514,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1522,7 +1526,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1534,7 +1538,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1546,7 +1550,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1558,7 +1562,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1570,7 +1574,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1582,7 +1586,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1594,7 +1598,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1606,7 +1610,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1618,7 +1622,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1630,7 +1634,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1642,7 +1646,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1654,7 +1658,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1666,7 +1670,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1678,7 +1682,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1690,7 +1694,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1702,7 +1706,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1714,7 +1718,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1726,7 +1730,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1738,7 +1742,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1750,7 +1754,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1762,7 +1766,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1774,7 +1778,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1786,7 +1790,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1798,7 +1802,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1810,7 +1814,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1822,7 +1826,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1834,7 +1838,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1846,7 +1850,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1858,7 +1862,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1870,7 +1874,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1882,7 +1886,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1894,7 +1898,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1906,7 +1910,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1918,7 +1922,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1930,7 +1934,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1942,7 +1946,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1954,7 +1958,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1966,7 +1970,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1978,7 +1982,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1990,7 +1994,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2002,7 +2006,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2014,7 +2018,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2026,7 +2030,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2038,7 +2042,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2050,7 +2054,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2062,7 +2066,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2074,7 +2078,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2086,7 +2090,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2098,7 +2102,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2110,7 +2114,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2122,7 +2126,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2134,7 +2138,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2146,7 +2150,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2158,7 +2162,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2170,7 +2174,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2182,7 +2186,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2194,7 +2198,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2206,7 +2210,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2218,7 +2222,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2230,7 +2234,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2242,7 +2246,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2254,7 +2258,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2266,7 +2270,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2278,7 +2282,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2290,7 +2294,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2302,7 +2306,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2314,7 +2318,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2326,7 +2330,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2338,7 +2342,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2350,7 +2354,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2362,7 +2366,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2374,7 +2378,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2386,7 +2390,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2398,7 +2402,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2410,7 +2414,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2422,7 +2426,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2434,7 +2438,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2446,7 +2450,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2458,7 +2462,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2470,7 +2474,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2482,7 +2486,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2494,7 +2498,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2506,7 +2510,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2518,7 +2522,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2530,7 +2534,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2542,7 +2546,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2554,7 +2558,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2566,7 +2570,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2578,7 +2582,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
@@ -2590,7 +2594,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
@@ -2602,7 +2606,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
@@ -2614,7 +2618,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
@@ -2626,7 +2630,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
@@ -2638,7 +2642,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
@@ -2650,7 +2654,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
@@ -2662,7 +2666,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
@@ -2675,30 +2679,30 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C109"/>
+  <autoFilter ref="A1:C109" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView topLeftCell="D16" workbookViewId="0">
       <selection activeCell="E53" sqref="E1:F53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" style="1"/>
-    <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="1"/>
-    <col min="5" max="5" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.5703125" style="1"/>
+    <col min="1" max="2" width="11.5546875" style="1"/>
+    <col min="3" max="3" width="11.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="1"/>
+    <col min="5" max="5" width="24.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="s">
         <v>158</v>
       </c>
@@ -2710,7 +2714,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>106</v>
       </c>
@@ -2731,7 +2735,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>107</v>
       </c>
@@ -2752,7 +2756,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>108</v>
       </c>
@@ -2773,7 +2777,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>109</v>
       </c>
@@ -2794,7 +2798,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>110</v>
       </c>
@@ -2815,7 +2819,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>111</v>
       </c>
@@ -2836,7 +2840,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>112</v>
       </c>
@@ -2857,7 +2861,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>113</v>
       </c>
@@ -2878,7 +2882,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>114</v>
       </c>
@@ -2899,7 +2903,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>115</v>
       </c>
@@ -2920,7 +2924,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>116</v>
       </c>
@@ -2941,7 +2945,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>117</v>
       </c>
@@ -2962,7 +2966,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>118</v>
       </c>
@@ -2983,7 +2987,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>119</v>
       </c>
@@ -3004,7 +3008,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>120</v>
       </c>
@@ -3025,7 +3029,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>121</v>
       </c>
@@ -3046,7 +3050,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>122</v>
       </c>
@@ -3067,7 +3071,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>123</v>
       </c>
@@ -3088,7 +3092,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>124</v>
       </c>
@@ -3109,7 +3113,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>125</v>
       </c>
@@ -3130,7 +3134,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>126</v>
       </c>
@@ -3151,7 +3155,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>127</v>
       </c>
@@ -3172,7 +3176,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>128</v>
       </c>
@@ -3193,7 +3197,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>129</v>
       </c>
@@ -3214,7 +3218,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>130</v>
       </c>
@@ -3235,7 +3239,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>131</v>
       </c>
@@ -3256,7 +3260,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>132</v>
       </c>
@@ -3277,7 +3281,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>133</v>
       </c>
@@ -3298,7 +3302,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>134</v>
       </c>
@@ -3319,7 +3323,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>135</v>
       </c>
@@ -3340,7 +3344,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>136</v>
       </c>
@@ -3361,7 +3365,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>137</v>
       </c>
@@ -3382,7 +3386,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>138</v>
       </c>
@@ -3403,7 +3407,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>139</v>
       </c>
@@ -3424,7 +3428,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>140</v>
       </c>
@@ -3445,7 +3449,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>141</v>
       </c>
@@ -3466,7 +3470,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>142</v>
       </c>
@@ -3487,7 +3491,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>143</v>
       </c>
@@ -3508,7 +3512,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>144</v>
       </c>
@@ -3529,7 +3533,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>145</v>
       </c>
@@ -3550,7 +3554,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>146</v>
       </c>
@@ -3571,7 +3575,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>147</v>
       </c>
@@ -3592,7 +3596,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>148</v>
       </c>
@@ -3613,7 +3617,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>149</v>
       </c>
@@ -3634,7 +3638,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>150</v>
       </c>
@@ -3655,7 +3659,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>151</v>
       </c>
@@ -3676,7 +3680,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>152</v>
       </c>
@@ -3697,7 +3701,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>153</v>
       </c>
@@ -3718,7 +3722,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>154</v>
       </c>
@@ -3739,7 +3743,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>155</v>
       </c>
@@ -3760,7 +3764,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>156</v>
       </c>
@@ -3781,7 +3785,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>157</v>
       </c>

</xml_diff>